<commit_message>
Add 2.0.0 version features
</commit_message>
<xml_diff>
--- a/Players Sample.xlsx
+++ b/Players Sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27030"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EB65E9E-923C-4038-B758-C29001AE069C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C80BFC7-31DD-461F-A3CE-CD74DC060B70}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Identifier</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -516,22 +513,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,255 +538,195 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="B19">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="B20">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>

</xml_diff>